<commit_message>
add fixed lead option
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/matlabTuning.xlsx
+++ b/myESC-Particle-DEV/saves/matlabTuning.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\GitHub\ESC\myESC-Particle-DEV\saves\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19650" windowHeight="8385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20976" windowHeight="8400"/>
   </bookViews>
   <sheets>
     <sheet name="Retune 20161102" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -56,9 +61,6 @@
   </si>
   <si>
     <t>Design LG, r/s</t>
-  </si>
-  <si>
-    <t>Entries for potESC.ino Arduino</t>
   </si>
   <si>
     <t>TauT, s</t>
@@ -154,13 +156,16 @@
     <t>E.TauE=0.1, tldF=0.15,tlgF=0.03, Step</t>
   </si>
   <si>
-    <t>Entries for potESC.ino Arduino   FIXED LEAD</t>
-  </si>
-  <si>
     <t>Design LG FIXED, r/s</t>
   </si>
   <si>
     <t>Design tld FIXED, s</t>
+  </si>
+  <si>
+    <t>Entries for potESC.ino FIXED LEAD</t>
+  </si>
+  <si>
+    <t>Entries for potESC.ino</t>
   </si>
 </sst>
 </file>
@@ -544,8 +549,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215125376"/>
-        <c:axId val="215135744"/>
+        <c:axId val="106091272"/>
+        <c:axId val="106086960"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -713,11 +718,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215152128"/>
-        <c:axId val="215137664"/>
+        <c:axId val="106088528"/>
+        <c:axId val="106088136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="215125376"/>
+        <c:axId val="106091272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -747,12 +752,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215135744"/>
+        <c:crossAx val="106086960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215135744"/>
+        <c:axId val="106086960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -788,12 +793,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215125376"/>
+        <c:crossAx val="106091272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215137664"/>
+        <c:axId val="106088136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -823,12 +828,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215152128"/>
+        <c:crossAx val="106088528"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215152128"/>
+        <c:axId val="106088528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,7 +843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215137664"/>
+        <c:crossAx val="106088136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1092,8 +1097,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215200896"/>
-        <c:axId val="215202816"/>
+        <c:axId val="106089704"/>
+        <c:axId val="106090096"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1261,11 +1266,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215206912"/>
-        <c:axId val="215204992"/>
+        <c:axId val="106090880"/>
+        <c:axId val="106090488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="215200896"/>
+        <c:axId val="106089704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -1288,19 +1293,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215202816"/>
+        <c:crossAx val="106090096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215202816"/>
+        <c:axId val="106090096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -1329,19 +1333,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215200896"/>
+        <c:crossAx val="106089704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215204992"/>
+        <c:axId val="106090488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1365,19 +1368,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215206912"/>
+        <c:crossAx val="106090880"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215206912"/>
+        <c:axId val="106090880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215204992"/>
+        <c:crossAx val="106090488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1641,8 +1643,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215263872"/>
-        <c:axId val="215270144"/>
+        <c:axId val="107007896"/>
+        <c:axId val="541418096"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1810,11 +1812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215278336"/>
-        <c:axId val="215272064"/>
+        <c:axId val="541421232"/>
+        <c:axId val="541416920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="215263872"/>
+        <c:axId val="107007896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1844,12 +1846,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215270144"/>
+        <c:crossAx val="541418096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215270144"/>
+        <c:axId val="541418096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -1885,12 +1887,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215263872"/>
+        <c:crossAx val="107007896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215272064"/>
+        <c:axId val="541416920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1920,12 +1922,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215278336"/>
+        <c:crossAx val="541421232"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215278336"/>
+        <c:axId val="541421232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1935,7 +1937,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215272064"/>
+        <c:crossAx val="541416920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2189,8 +2191,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215318912"/>
-        <c:axId val="215320832"/>
+        <c:axId val="541422408"/>
+        <c:axId val="541418488"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2358,11 +2360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="215329024"/>
-        <c:axId val="215327104"/>
+        <c:axId val="541415744"/>
+        <c:axId val="541421624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="215318912"/>
+        <c:axId val="541422408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -2385,19 +2387,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215320832"/>
+        <c:crossAx val="541418488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215320832"/>
+        <c:axId val="541418488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -2426,19 +2427,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215318912"/>
+        <c:crossAx val="541422408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215327104"/>
+        <c:axId val="541421624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -2462,19 +2462,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215329024"/>
+        <c:crossAx val="541415744"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="215329024"/>
+        <c:axId val="541415744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2484,7 +2483,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="215327104"/>
+        <c:crossAx val="541421624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2738,8 +2737,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115506176"/>
-        <c:axId val="116655232"/>
+        <c:axId val="541422800"/>
+        <c:axId val="541416528"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2907,11 +2906,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116667520"/>
-        <c:axId val="116657152"/>
+        <c:axId val="541423192"/>
+        <c:axId val="541420056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115506176"/>
+        <c:axId val="541422800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -2941,12 +2940,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116655232"/>
+        <c:crossAx val="541416528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116655232"/>
+        <c:axId val="541416528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -2982,12 +2981,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115506176"/>
+        <c:crossAx val="541422800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116657152"/>
+        <c:axId val="541420056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -3017,12 +3016,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116667520"/>
+        <c:crossAx val="541423192"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116667520"/>
+        <c:axId val="541423192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3032,7 +3031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116657152"/>
+        <c:crossAx val="541420056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3291,8 +3290,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116728576"/>
-        <c:axId val="116730496"/>
+        <c:axId val="541420840"/>
+        <c:axId val="541418880"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3460,11 +3459,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116750976"/>
-        <c:axId val="116749056"/>
+        <c:axId val="541417704"/>
+        <c:axId val="541417312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116728576"/>
+        <c:axId val="541420840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -3494,12 +3493,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116730496"/>
+        <c:crossAx val="541418880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116730496"/>
+        <c:axId val="541418880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -3535,12 +3534,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116728576"/>
+        <c:crossAx val="541420840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116749056"/>
+        <c:axId val="541417312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -3570,12 +3569,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116750976"/>
+        <c:crossAx val="541417704"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116750976"/>
+        <c:axId val="541417704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3585,7 +3584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116749056"/>
+        <c:crossAx val="541417312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3950,7 +3949,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3985,7 +3984,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4197,42 +4196,42 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:X111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="P88" sqref="P88"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="7.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
     </row>
-    <row r="2" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4246,10 +4245,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>4</v>
@@ -4282,18 +4281,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="18">
         <v>0.35</v>
@@ -4336,18 +4335,18 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="18">
         <v>0.3</v>
@@ -4390,18 +4389,18 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="18">
         <v>0.2</v>
@@ -4434,18 +4433,18 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="18">
         <v>0.1</v>
@@ -4488,18 +4487,18 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="18">
         <v>0.05</v>
@@ -4542,18 +4541,18 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="18">
         <v>0.02</v>
@@ -4596,21 +4595,21 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="10" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>2</v>
@@ -4619,10 +4618,10 @@
         <v>3</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>4</v>
@@ -4655,30 +4654,30 @@
         <v>13</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="9">
         <v>16</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="18">
         <v>0.34399999999999997</v>
@@ -4736,18 +4735,18 @@
         <v>4.5579999999999996E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="9">
         <v>19</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="18">
         <v>0.28999999999999998</v>
@@ -4774,18 +4773,18 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="5"/>
     </row>
-    <row r="14" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="9">
         <v>25</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="18">
         <v>0.185</v>
@@ -4843,18 +4842,18 @@
         <v>2.035E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="9">
         <v>47</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="18">
         <v>8.5000000000000006E-2</v>
@@ -4912,18 +4911,18 @@
         <v>7.4374999999999997E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="9">
         <v>61</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="18">
         <v>0.04</v>
@@ -4950,18 +4949,18 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="5"/>
     </row>
-    <row r="17" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="9">
         <v>70</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="18">
         <v>0.02</v>
@@ -5019,24 +5018,24 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="R18" s="5"/>
     </row>
-    <row r="19" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H19" s="9"/>
     </row>
-    <row r="20" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>2</v>
@@ -5045,10 +5044,10 @@
         <v>3</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>4</v>
@@ -5075,36 +5074,36 @@
         <v>11</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="T20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="9">
         <v>16</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="18">
         <v>0.34399999999999997</v>
@@ -5162,18 +5161,18 @@
         <v>2.3220000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="9">
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="18">
         <v>0.28999999999999998</v>
@@ -5200,18 +5199,18 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="5"/>
     </row>
-    <row r="23" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="9">
         <v>25</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" s="18">
         <v>0.185</v>
@@ -5253,7 +5252,7 @@
         <v>3.8174999999999999</v>
       </c>
       <c r="Q23" s="4">
-        <f t="shared" ref="Q23:Q26" si="9">I23*H23</f>
+        <f t="shared" ref="Q23:Q24" si="9">I23*H23</f>
         <v>0.92390909750962025</v>
       </c>
       <c r="R23" s="5">
@@ -5265,22 +5264,22 @@
         <v>0.33783783783783783</v>
       </c>
       <c r="T23" s="1">
-        <f t="shared" ref="T23:T26" si="11">R23*E23</f>
+        <f t="shared" ref="T23:T24" si="11">R23*E23</f>
         <v>1.15625E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="9">
         <v>47</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="18">
         <v>8.5000000000000006E-2</v>
@@ -5338,18 +5337,18 @@
         <v>4.6750000000000003E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="9">
         <v>61</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25" s="18">
         <v>0.04</v>
@@ -5376,18 +5375,18 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="5"/>
     </row>
-    <row r="26" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="9">
         <v>70</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" s="18">
         <v>0.02</v>
@@ -5429,7 +5428,7 @@
         <v>5.0128000000000004</v>
       </c>
       <c r="Q26" s="4">
-        <f t="shared" ref="Q26:Q27" si="12">I26*H26</f>
+        <f t="shared" ref="Q26" si="12">I26*H26</f>
         <v>0.46518188567186347</v>
       </c>
       <c r="R26" s="5">
@@ -5441,32 +5440,32 @@
         <v>1.7500000000000002</v>
       </c>
       <c r="T26" s="1">
-        <f t="shared" ref="T26:T27" si="13">R26*E26</f>
+        <f t="shared" ref="T26" si="13">R26*E26</f>
         <v>7.000000000000001E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="R27" s="5"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="R28" s="5"/>
     </row>
-    <row r="29" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="H29" s="9"/>
       <c r="R29" s="5"/>
     </row>
-    <row r="30" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>2</v>
@@ -5475,13 +5474,13 @@
         <v>3</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>5</v>
@@ -5508,18 +5507,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="9">
         <v>16</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E31" s="18">
         <v>0.34399999999999997</v>
@@ -5547,18 +5546,18 @@
       </c>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="9">
         <v>19</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E32" s="18">
         <v>0.28999999999999998</v>
@@ -5586,18 +5585,18 @@
       </c>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="9">
         <v>25</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E33" s="18">
         <v>0.185</v>
@@ -5625,18 +5624,18 @@
       </c>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34" s="9">
         <v>47</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E34" s="18">
         <v>8.5000000000000006E-2</v>
@@ -5664,18 +5663,18 @@
       </c>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B35" s="9">
         <v>61</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E35" s="18">
         <v>0.04</v>
@@ -5703,18 +5702,18 @@
       </c>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B36" s="9">
         <v>70</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E36" s="18">
         <v>0.02</v>
@@ -5742,7 +5741,7 @@
       </c>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -5762,17 +5761,17 @@
       <c r="Q37" s="5"/>
       <c r="R37" s="5"/>
     </row>
-    <row r="38" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B38" s="1" t="s">
-        <v>14</v>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="S38" s="7"/>
       <c r="T38" s="7"/>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="6">
         <f>Q52</f>
@@ -5802,9 +5801,9 @@
       <c r="T39" s="7"/>
       <c r="U39" s="7"/>
     </row>
-    <row r="40" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" s="6">
         <f>S52</f>
@@ -5834,9 +5833,9 @@
       <c r="T40" s="20"/>
       <c r="U40" s="7"/>
     </row>
-    <row r="41" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" s="23">
         <f>R52</f>
@@ -5866,14 +5865,14 @@
       <c r="T41" s="20"/>
       <c r="U41" s="7"/>
     </row>
-    <row r="42" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="S42" s="19"/>
       <c r="T42" s="20"/>
       <c r="U42" s="7"/>
     </row>
-    <row r="43" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43" s="6">
         <f>P57</f>
@@ -5903,9 +5902,9 @@
       <c r="T43" s="20"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="44" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" s="6">
         <f>S57</f>
@@ -5935,9 +5934,9 @@
       <c r="T44" s="20"/>
       <c r="U44" s="7"/>
     </row>
-    <row r="45" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" s="23">
         <f>R57</f>
@@ -5967,17 +5966,17 @@
       <c r="T45" s="20"/>
       <c r="U45" s="7"/>
     </row>
-    <row r="46" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="S46" s="19"/>
       <c r="T46" s="20"/>
       <c r="U46" s="7"/>
     </row>
-    <row r="47" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="S47" s="19"/>
       <c r="T47" s="20"/>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -5989,7 +5988,7 @@
       <c r="T48" s="20"/>
       <c r="U48" s="7"/>
     </row>
-    <row r="49" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -6001,29 +6000,29 @@
       <c r="T49" s="20"/>
       <c r="U49" s="7"/>
     </row>
-    <row r="50" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P50" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q50" s="9"/>
       <c r="R50" s="9"/>
       <c r="S50" s="9"/>
     </row>
-    <row r="51" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P51" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R51" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R51" s="1" t="s">
+      <c r="S51" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S51" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P52" s="9">
         <v>78</v>
       </c>
@@ -6037,7 +6036,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="53" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P53" s="9">
         <v>62</v>
       </c>
@@ -6051,7 +6050,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="54" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P54" s="9">
         <v>47.5</v>
       </c>
@@ -6065,7 +6064,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P55" s="9">
         <v>25</v>
       </c>
@@ -6079,7 +6078,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="56" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P56" s="9">
         <v>16</v>
       </c>
@@ -6093,7 +6092,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="57" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P57" s="9">
         <v>0</v>
       </c>
@@ -6107,30 +6106,30 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="59" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="V59" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="V60" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W60" s="9"/>
       <c r="X60" s="9"/>
     </row>
-    <row r="61" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="V61" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="W61" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="W61" s="21" t="s">
-        <v>35</v>
-      </c>
       <c r="X61" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="V62" s="24">
         <v>0.34399999999999997</v>
       </c>
@@ -6141,7 +6140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="V63" s="24">
         <v>0.27100000000000002</v>
       </c>
@@ -6152,9 +6151,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B64" s="1" t="s">
-        <v>46</v>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A64" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="S64" s="7"/>
       <c r="V64" s="24">
@@ -6167,9 +6166,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B65" s="6">
         <f>Q78</f>
@@ -6206,9 +6205,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B66" s="6">
         <f>S78</f>
@@ -6245,9 +6244,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B67" s="23">
         <f>R78</f>
@@ -6284,7 +6283,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S68" s="19"/>
       <c r="V68" s="24">
         <v>6.4000000000000001E-2</v>
@@ -6296,9 +6295,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B69" s="6">
         <f>P83</f>
@@ -6335,9 +6334,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B70" s="6">
         <f>S83</f>
@@ -6374,9 +6373,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B71" s="23">
         <f>R83</f>
@@ -6404,13 +6403,13 @@
       </c>
       <c r="S71" s="19"/>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S72" s="19"/>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S73" s="19"/>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -6420,7 +6419,7 @@
       <c r="G74" s="7"/>
       <c r="S74" s="19"/>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -6430,29 +6429,29 @@
       <c r="G75" s="7"/>
       <c r="S75" s="19"/>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P76" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q76" s="9"/>
       <c r="R76" s="9"/>
       <c r="S76" s="9"/>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P77" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R77" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R77" s="1" t="s">
+      <c r="S77" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S77" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P78" s="9">
         <v>78</v>
       </c>
@@ -6466,7 +6465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P79" s="9">
         <v>62</v>
       </c>
@@ -6480,7 +6479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="P80" s="9">
         <v>47.5</v>
       </c>
@@ -6494,7 +6493,7 @@
         <v>4.05</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P81" s="9">
         <v>25</v>
       </c>
@@ -6508,7 +6507,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P82" s="9">
         <v>16</v>
       </c>
@@ -6522,7 +6521,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P83" s="9">
         <v>0</v>
       </c>
@@ -6536,14 +6535,14 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B93" s="6">
         <f>Q106</f>
@@ -6570,9 +6569,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B94" s="6">
         <f>S106</f>
@@ -6599,9 +6598,9 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B95" s="23">
         <f>R106</f>
@@ -6628,9 +6627,9 @@
         <v>0.48799999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B97" s="6">
         <f>P111</f>
@@ -6657,9 +6656,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B98" s="6">
         <f>S111</f>
@@ -6686,9 +6685,9 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B99" s="23">
         <f>R111</f>
@@ -6715,29 +6714,29 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P104" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q104" s="9"/>
       <c r="R104" s="9"/>
       <c r="S104" s="9"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P105" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q105" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R105" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S105" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S105" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P106" s="9">
         <v>80</v>
       </c>
@@ -6751,7 +6750,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P107" s="9">
         <v>62</v>
       </c>
@@ -6765,7 +6764,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P108" s="9">
         <v>47.5</v>
       </c>
@@ -6779,7 +6778,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P109" s="9">
         <v>25</v>
       </c>
@@ -6793,7 +6792,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P110" s="9">
         <v>16</v>
       </c>
@@ -6807,7 +6806,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="P111" s="9">
         <v>0</v>
       </c>

</xml_diff>